<commit_message>
[experiments][suricata] More graphs about 512MB test.
</commit_message>
<xml_diff>
--- a/experiments/suricata/data/bigFlows.pcap,1-4,eve.xlsx
+++ b/experiments/suricata/data/bigFlows.pcap,1-4,eve.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Capture" sheetId="2" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>1xBM,Decode.Pkts</t>
   </si>
   <si>
-    <t>1xBM,Decode.Bytes</t>
-  </si>
-  <si>
     <t>2xBM,Capture.Pkts</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>2xBM,Decode.Pkts</t>
-  </si>
-  <si>
-    <t>2xBM,Decode.Bytes</t>
   </si>
   <si>
     <t>3xBM,Capture.Pkts</t>
@@ -77,9 +71,6 @@
     <t>3xBM,Decode.Pkts</t>
   </si>
   <si>
-    <t>3xBM,Decode.Bytes</t>
-  </si>
-  <si>
     <t>4xBM,Capture.Pkts</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
   </si>
   <si>
     <t>4xBM,Decode.Pkts</t>
-  </si>
-  <si>
-    <t>4xBM,Decode.Bytes</t>
   </si>
   <si>
     <t>1xDocker,Capture.Pkts</t>
@@ -101,9 +89,6 @@
     <t>1xDocker,Decode.Pkts</t>
   </si>
   <si>
-    <t>1xDocker,Decode.Bytes</t>
-  </si>
-  <si>
     <t>2xDocker,Capture.Pkts</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
   </si>
   <si>
     <t>2xDocker,Decode.Pkts</t>
-  </si>
-  <si>
-    <t>2xDocker,Decode.Bytes</t>
   </si>
   <si>
     <t>3xDocker,Capture.Pkts</t>
@@ -125,9 +107,6 @@
     <t>3xDocker,Decode.Pkts</t>
   </si>
   <si>
-    <t>3xDocker,Decode.Bytes</t>
-  </si>
-  <si>
     <t>4xDocker,Capture.Pkts</t>
   </si>
   <si>
@@ -135,9 +114,6 @@
   </si>
   <si>
     <t>4xDocker,Decode.Pkts</t>
-  </si>
-  <si>
-    <t>4xDocker,Decode.Bytes</t>
   </si>
   <si>
     <t>1xDockerV,Capture.Pkts</t>
@@ -149,9 +125,6 @@
     <t>1xDockerV,Decode.Pkts</t>
   </si>
   <si>
-    <t>1xDockerV,Decode.Bytes</t>
-  </si>
-  <si>
     <t>2xDockerV,Capture.Pkts</t>
   </si>
   <si>
@@ -159,9 +132,6 @@
   </si>
   <si>
     <t>2xDockerV,Decode.Pkts</t>
-  </si>
-  <si>
-    <t>2xDockerV,Decode.Bytes</t>
   </si>
   <si>
     <t>3xDockerV,Capture.Pkts</t>
@@ -173,9 +143,6 @@
     <t>3xDockerV,Decode.Pkts</t>
   </si>
   <si>
-    <t>3xDockerV,Decode.Bytes</t>
-  </si>
-  <si>
     <t>4xDockerV,Capture.Pkts</t>
   </si>
   <si>
@@ -183,9 +150,6 @@
   </si>
   <si>
     <t>4xDockerV,Decode.Pkts</t>
-  </si>
-  <si>
-    <t>4xDockerV,Decode.Bytes</t>
   </si>
   <si>
     <t>1xKVM,Capture.Pkts</t>
@@ -197,9 +161,6 @@
     <t>1xKVM,Decode.Pkts</t>
   </si>
   <si>
-    <t>1xKVM,Decode.Bytes</t>
-  </si>
-  <si>
     <t>2xKVM,Capture.Pkts</t>
   </si>
   <si>
@@ -207,9 +168,6 @@
   </si>
   <si>
     <t>2xKVM,Decode.Pkts</t>
-  </si>
-  <si>
-    <t>2xKVM,Decode.Bytes</t>
   </si>
   <si>
     <t>3xKVM,Capture.Pkts</t>
@@ -221,9 +179,6 @@
     <t>3xKVM,Decode.Pkts</t>
   </si>
   <si>
-    <t>3xKVM,Decode.Bytes</t>
-  </si>
-  <si>
     <t>4xKVM,Capture.Pkts</t>
   </si>
   <si>
@@ -233,10 +188,55 @@
     <t>4xKVM,Decode.Pkts</t>
   </si>
   <si>
-    <t>4xKVM,Decode.Bytes</t>
+    <t>Uptime</t>
   </si>
   <si>
-    <t>Uptime</t>
+    <t>1xBM,Decode.KB</t>
+  </si>
+  <si>
+    <t>2xBM,Decode.KB</t>
+  </si>
+  <si>
+    <t>3xBM,Decode.KB</t>
+  </si>
+  <si>
+    <t>4xBM,Decode.KB</t>
+  </si>
+  <si>
+    <t>1xDocker,Decode.KB</t>
+  </si>
+  <si>
+    <t>2xDocker,Decode.KB</t>
+  </si>
+  <si>
+    <t>3xDocker,Decode.KB</t>
+  </si>
+  <si>
+    <t>4xDocker,Decode.KB</t>
+  </si>
+  <si>
+    <t>1xDockerV,Decode.KB</t>
+  </si>
+  <si>
+    <t>2xDockerV,Decode.KB</t>
+  </si>
+  <si>
+    <t>3xDockerV,Decode.KB</t>
+  </si>
+  <si>
+    <t>4xDockerV,Decode.KB</t>
+  </si>
+  <si>
+    <t>1xKVM,Decode.KB</t>
+  </si>
+  <si>
+    <t>2xKVM,Decode.KB</t>
+  </si>
+  <si>
+    <t>3xKVM,Decode.KB</t>
+  </si>
+  <si>
+    <t>4xKVM,Decode.KB</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5586,7 +5585,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5707,7 +5705,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5782,7 +5779,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5900,7 +5896,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11141,7 +11136,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11262,7 +11256,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11337,7 +11330,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11455,7 +11447,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15408,7 +15399,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15529,7 +15519,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15604,7 +15593,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15722,7 +15710,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18377,7 +18364,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18498,7 +18484,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18573,7 +18558,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18736,7 +18720,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1xBM,Decode.Bytes</c:v>
+                  <c:v>1xBM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19057,7 +19041,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2xBM,Decode.Bytes</c:v>
+                  <c:v>2xBM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19378,7 +19362,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3xBM,Decode.Bytes</c:v>
+                  <c:v>3xBM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19699,7 +19683,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4xBM,Decode.Bytes</c:v>
+                  <c:v>4xBM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -20020,7 +20004,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1xKVM,Decode.Bytes</c:v>
+                  <c:v>1xKVM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -20341,7 +20325,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2xKVM,Decode.Bytes</c:v>
+                  <c:v>2xKVM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -20664,7 +20648,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3xKVM,Decode.Bytes</c:v>
+                  <c:v>3xKVM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -20987,7 +20971,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4xKVM,Decode.Bytes</c:v>
+                  <c:v>4xKVM,Decode.KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -24436,7 +24420,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -24556,7 +24540,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660423" cy="6286500"/>
+    <xdr:ext cx="8656320" cy="6278880"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -36396,13 +36380,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -36414,190 +36400,190 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AC1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AF1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AG1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AI1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AK1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AM1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AN1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AO1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AQ1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AR1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AS1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AU1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AV1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AW1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AY1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AZ1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BA1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BC1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BD1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BE1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BG1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BH1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BI1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BK1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BL1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>62</v>
-      </c>
       <c r="BM1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>8</v>
       </c>
@@ -36858,7 +36844,7 @@
         <v>20811.3876953125</v>
       </c>
     </row>
-    <row r="3" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>16</v>
       </c>
@@ -37119,7 +37105,7 @@
         <v>34734.3603515625</v>
       </c>
     </row>
-    <row r="4" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>24</v>
       </c>
@@ -37380,7 +37366,7 @@
         <v>48195.2333984375</v>
       </c>
     </row>
-    <row r="5" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>32</v>
       </c>
@@ -37641,7 +37627,7 @@
         <v>62828.548828125</v>
       </c>
     </row>
-    <row r="6" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>40</v>
       </c>
@@ -37902,7 +37888,7 @@
         <v>78276.373046875</v>
       </c>
     </row>
-    <row r="7" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>48</v>
       </c>
@@ -38163,7 +38149,7 @@
         <v>91439.396484375</v>
       </c>
     </row>
-    <row r="8" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>56</v>
       </c>
@@ -38424,7 +38410,7 @@
         <v>104602.833984375</v>
       </c>
     </row>
-    <row r="9" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>64</v>
       </c>
@@ -38685,7 +38671,7 @@
         <v>112986.6005859375</v>
       </c>
     </row>
-    <row r="10" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>72</v>
       </c>
@@ -38946,7 +38932,7 @@
         <v>124570.1318359375</v>
       </c>
     </row>
-    <row r="11" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>80</v>
       </c>
@@ -39207,7 +39193,7 @@
         <v>137166.7236328125</v>
       </c>
     </row>
-    <row r="12" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>88</v>
       </c>
@@ -39468,7 +39454,7 @@
         <v>150664.310546875</v>
       </c>
     </row>
-    <row r="13" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>96</v>
       </c>
@@ -39729,7 +39715,7 @@
         <v>163854.3720703125</v>
       </c>
     </row>
-    <row r="14" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>104</v>
       </c>
@@ -39990,7 +39976,7 @@
         <v>175984.3251953125</v>
       </c>
     </row>
-    <row r="15" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>112</v>
       </c>
@@ -40251,7 +40237,7 @@
         <v>183701.38671875</v>
       </c>
     </row>
-    <row r="16" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>120</v>
       </c>
@@ -40512,7 +40498,7 @@
         <v>196954.2080078125</v>
       </c>
     </row>
-    <row r="17" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>128</v>
       </c>
@@ -40773,7 +40759,7 @@
         <v>210138.7080078125</v>
       </c>
     </row>
-    <row r="18" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>136</v>
       </c>
@@ -41034,7 +41020,7 @@
         <v>225492.9658203125</v>
       </c>
     </row>
-    <row r="19" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>144</v>
       </c>
@@ -41295,7 +41281,7 @@
         <v>238933.947265625</v>
       </c>
     </row>
-    <row r="20" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>152</v>
       </c>
@@ -41556,7 +41542,7 @@
         <v>250649.65625</v>
       </c>
     </row>
-    <row r="21" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>160</v>
       </c>
@@ -41817,7 +41803,7 @@
         <v>269580.8193359375</v>
       </c>
     </row>
-    <row r="22" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>168</v>
       </c>
@@ -42078,7 +42064,7 @@
         <v>286951.3515625</v>
       </c>
     </row>
-    <row r="23" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>176</v>
       </c>
@@ -42339,7 +42325,7 @@
         <v>299480.123046875</v>
       </c>
     </row>
-    <row r="24" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>184</v>
       </c>
@@ -42600,7 +42586,7 @@
         <v>314098.2314453125</v>
       </c>
     </row>
-    <row r="25" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>192</v>
       </c>
@@ -42861,7 +42847,7 @@
         <v>328612.806640625</v>
       </c>
     </row>
-    <row r="26" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>200</v>
       </c>
@@ -43122,7 +43108,7 @@
         <v>339694.1474609375</v>
       </c>
     </row>
-    <row r="27" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>208</v>
       </c>
@@ -43383,7 +43369,7 @@
         <v>349520.0302734375</v>
       </c>
     </row>
-    <row r="28" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>216</v>
       </c>
@@ -43644,7 +43630,7 @@
         <v>360875.1396484375</v>
       </c>
     </row>
-    <row r="29" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>224</v>
       </c>
@@ -43905,7 +43891,7 @@
         <v>372150.7744140625</v>
       </c>
     </row>
-    <row r="30" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>232</v>
       </c>
@@ -44166,7 +44152,7 @@
         <v>384447.875</v>
       </c>
     </row>
-    <row r="31" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>240</v>
       </c>
@@ -44427,7 +44413,7 @@
         <v>394745.28125</v>
       </c>
     </row>
-    <row r="32" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>248</v>
       </c>
@@ -44688,7 +44674,7 @@
         <v>405505.5029296875</v>
       </c>
     </row>
-    <row r="33" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>256</v>
       </c>
@@ -44949,7 +44935,7 @@
         <v>416876.767578125</v>
       </c>
     </row>
-    <row r="34" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>264</v>
       </c>
@@ -45210,7 +45196,7 @@
         <v>429210.0302734375</v>
       </c>
     </row>
-    <row r="35" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>272</v>
       </c>
@@ -45471,7 +45457,7 @@
         <v>439975.42578125</v>
       </c>
     </row>
-    <row r="36" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>280</v>
       </c>
@@ -45732,7 +45718,7 @@
         <v>452567.8369140625</v>
       </c>
     </row>
-    <row r="37" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>288</v>
       </c>
@@ -45993,7 +45979,7 @@
         <v>463090.8876953125</v>
       </c>
     </row>
-    <row r="38" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>296</v>
       </c>
@@ -46254,7 +46240,7 @@
         <v>476218.9658203125</v>
       </c>
     </row>
-    <row r="39" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>304</v>
       </c>
@@ -46515,7 +46501,7 @@
         <v>486796.25</v>
       </c>
     </row>
-    <row r="40" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>312</v>
       </c>
@@ -46776,7 +46762,7 @@
         <v>501050.3447265625</v>
       </c>
     </row>
-    <row r="41" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>320</v>
       </c>
@@ -47037,7 +47023,7 @@
         <v>516008.4111328125</v>
       </c>
     </row>
-    <row r="42" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>328</v>
       </c>
@@ -47298,7 +47284,7 @@
         <v>531338.1318359375</v>
       </c>
     </row>
-    <row r="43" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>336</v>
       </c>
@@ -47559,7 +47545,7 @@
         <v>545290.63671875</v>
       </c>
     </row>
-    <row r="44" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>344</v>
       </c>
@@ -47820,7 +47806,7 @@
         <v>547018.904296875</v>
       </c>
     </row>
-    <row r="45" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>352</v>
       </c>
@@ -48081,7 +48067,7 @@
         <v>546140.826171875</v>
       </c>
     </row>
-    <row r="46" spans="1:65" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>360</v>
       </c>

</xml_diff>